<commit_message>
Add updated file via upload
</commit_message>
<xml_diff>
--- a/workshop-intro-to-low-code-dataset.xlsx
+++ b/workshop-intro-to-low-code-dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea0cd9429cdefcd6/Speaking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="11_F25DC773A252ABDACC1048D1F1185E965BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F4FB5E6-61C7-4DA8-BF2B-3566079764BB}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="11_F25DC773A252ABDACC1048D1F1185E965BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD8B867-1227-428B-BDDC-0A173C828482}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="481">
   <si>
     <t>777 Brockton Avenue, Abington MA 2351</t>
   </si>
@@ -1531,6 +1531,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{214D576F-FFF1-4A80-8EDD-4E981EAE8FCE}" name="Table1" displayName="Table1" ref="A1:E235" totalsRowShown="0">
+  <autoFilter ref="A1:E235" xr:uid="{214D576F-FFF1-4A80-8EDD-4E981EAE8FCE}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F94F7781-E71C-4B7F-91FB-00FDAA5D97EC}" name="Attendee Name"/>
+    <tableColumn id="2" xr3:uid="{1B8DEDA6-D9E8-4234-B284-C52DE085AF9B}" name="Most Interested in Product"/>
+    <tableColumn id="3" xr3:uid="{A47E0916-F326-4E6A-BD15-A7EB81315DCB}" name="Opt-in for lunch"/>
+    <tableColumn id="4" xr3:uid="{336DA029-1BB0-4171-9C96-1D60B6A120A7}" name="Opt-in for raffle"/>
+    <tableColumn id="5" xr3:uid="{0B9C0135-0A24-4825-A61A-938CAD71DF9B}" name="Attendee Address"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1802,7 +1816,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="32.6328125" customWidth="1"/>
+    <col min="1" max="2" width="32.6328125" customWidth="1"/>
+    <col min="3" max="4" width="24.6328125" customWidth="1"/>
+    <col min="5" max="5" width="48.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1880,9 +1896,6 @@
       <c r="B5" t="s">
         <v>469</v>
       </c>
-      <c r="C5" t="s">
-        <v>476</v>
-      </c>
       <c r="D5" t="s">
         <v>475</v>
       </c>
@@ -5767,5 +5780,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>